<commit_message>
allow adding teams to groups in excel
</commit_message>
<xml_diff>
--- a/tests/data/sigil.xlsx
+++ b/tests/data/sigil.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/workspace/sigil/tests/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14880" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -15,6 +20,9 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -23,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
   <si>
     <t>firstname</t>
   </si>
@@ -198,17 +206,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -540,9 +553,9 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -565,7 +578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -588,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -611,7 +624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -642,25 +655,20 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -671,7 +679,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -682,7 +690,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -690,13 +698,16 @@
         <v>22</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -705,12 +716,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -721,7 +732,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -732,7 +743,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -740,7 +751,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -750,28 +761,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="C5" sqref="A5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -782,7 +788,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -793,7 +799,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -801,19 +807,25 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -825,7 +837,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
@@ -834,7 +846,7 @@
     <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -851,7 +863,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -868,7 +880,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -879,7 +891,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -887,10 +899,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>